<commit_message>
Adicionar notebook da terceira aula
</commit_message>
<xml_diff>
--- a/base de acoes_pura.xlsx
+++ b/base de acoes_pura.xlsx
@@ -4280,11 +4280,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="552746863"/>
-        <c:axId val="1505268708"/>
+        <c:axId val="1800378398"/>
+        <c:axId val="1690736435"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="552746863"/>
+        <c:axId val="1800378398"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4336,10 +4336,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1505268708"/>
+        <c:crossAx val="1690736435"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1505268708"/>
+        <c:axId val="1690736435"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4414,7 +4414,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="552746863"/>
+        <c:crossAx val="1800378398"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -4506,11 +4506,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="586517008"/>
-        <c:axId val="443046736"/>
+        <c:axId val="1462181198"/>
+        <c:axId val="1809224292"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="586517008"/>
+        <c:axId val="1462181198"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4562,10 +4562,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="443046736"/>
+        <c:crossAx val="1809224292"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="443046736"/>
+        <c:axId val="1809224292"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4640,7 +4640,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="586517008"/>
+        <c:crossAx val="1462181198"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4723,11 +4723,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="216774798"/>
-        <c:axId val="1891223593"/>
+        <c:axId val="680292255"/>
+        <c:axId val="1576141514"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="216774798"/>
+        <c:axId val="680292255"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -4779,10 +4779,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1891223593"/>
+        <c:crossAx val="1576141514"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1891223593"/>
+        <c:axId val="1576141514"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4857,7 +4857,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216774798"/>
+        <c:crossAx val="680292255"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -26733,7 +26733,10 @@
         <f>SUMIF(Principal!R:R,A13,Principal!O:O)</f>
         <v>6093288832</v>
       </c>
-      <c r="C13" s="33"/>
+      <c r="C13" s="33">
+        <f>SUMIFS(Principal!O:O,Principal!R:R,A13,Principal!P:P,"Subiu")</f>
+        <v>6093288832</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="36" t="str">

</xml_diff>